<commit_message>
l10n_se_sru_codes: Changed some data files
</commit_message>
<xml_diff>
--- a/l10n_se_sru_codes/extra/INK2_19-P1-exkl-version-2022-11-1.xlsx
+++ b/l10n_se_sru_codes/extra/INK2_19-P1-exkl-version-2022-11-1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="303">
   <si>
     <t xml:space="preserve">Inkomstdeklaration 2</t>
   </si>
@@ -699,23 +699,7 @@
     <t xml:space="preserve">496x, 498x</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Tar inte med </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Verdana"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">40xx-47xx eftersom den redan finns i 7511</t>
-    </r>
+    <t xml:space="preserve">Tar inte med 40xx-47xx eftersom den redan finns i 7511</t>
   </si>
   <si>
     <t xml:space="preserve">3.7</t>
@@ -784,6 +768,9 @@
     <t xml:space="preserve">– 80xx exkl. (807x, 808x)</t>
   </si>
   <si>
+    <t xml:space="preserve">Skippar 807x, 808x eftersom dem finns på 7521</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.13</t>
   </si>
   <si>
@@ -838,6 +825,9 @@
     <t xml:space="preserve">– 82xx exkl. (827x, 828x)</t>
   </si>
   <si>
+    <t xml:space="preserve">Skippar 827x, 828x eftersom dem finns på 7521</t>
+  </si>
+  <si>
     <t xml:space="preserve">3.16</t>
   </si>
   <si>
@@ -908,6 +898,12 @@
   </si>
   <si>
     <t xml:space="preserve">8810, 8811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8811</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skippar 8810 eftersom den finns på 7420</t>
   </si>
   <si>
     <t xml:space="preserve">3.23</t>
@@ -981,7 +977,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1067,11 +1063,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1390,8 +1381,8 @@
   </sheetPr>
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C88" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D110" activeCellId="0" sqref="D110"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A112" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D120" activeCellId="0" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.9921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2996,7 +2987,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="37" t="n">
         <v>7518</v>
       </c>
@@ -3005,29 +2996,30 @@
       <c r="D110" s="32" t="s">
         <v>235</v>
       </c>
-      <c r="E110" s="33" t="s">
-        <v>234</v>
-      </c>
+      <c r="E110" s="33"/>
       <c r="F110" s="29"/>
+      <c r="G110" s="3" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="37" t="n">
         <v>7415</v>
       </c>
       <c r="B111" s="42" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C111" s="43" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D111" s="35" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E111" s="38" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F111" s="29" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3037,12 +3029,12 @@
       <c r="B112" s="42"/>
       <c r="C112" s="43"/>
       <c r="D112" s="35" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="E112" s="38"/>
       <c r="F112" s="29"/>
       <c r="G112" s="3" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3050,16 +3042,16 @@
         <v>7423</v>
       </c>
       <c r="B113" s="42" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C113" s="43" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D113" s="32" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="E113" s="38" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F113" s="29"/>
     </row>
@@ -3070,7 +3062,7 @@
       <c r="B114" s="42"/>
       <c r="C114" s="43"/>
       <c r="D114" s="32" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="E114" s="15"/>
       <c r="F114" s="29"/>
@@ -3080,53 +3072,54 @@
         <v>7416</v>
       </c>
       <c r="B115" s="42" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C115" s="43" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D115" s="32" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E115" s="38" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F115" s="29" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="37" t="n">
         <v>7520</v>
       </c>
       <c r="B116" s="42"/>
       <c r="C116" s="43"/>
       <c r="D116" s="32" t="s">
-        <v>253</v>
-      </c>
-      <c r="E116" s="38" t="s">
-        <v>252</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="E116" s="38"/>
       <c r="F116" s="29"/>
+      <c r="G116" s="3" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="26.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="37" t="n">
         <v>7417</v>
       </c>
       <c r="B117" s="33" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C117" s="34" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D117" s="35" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="E117" s="38" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="F117" s="29" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="38.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3134,16 +3127,16 @@
         <v>7521</v>
       </c>
       <c r="B118" s="33" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C118" s="34" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D118" s="35" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="E118" s="38" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F118" s="29"/>
     </row>
@@ -3152,16 +3145,16 @@
         <v>7522</v>
       </c>
       <c r="B119" s="33" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C119" s="34" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D119" s="35" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="E119" s="38" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="F119" s="29"/>
     </row>
@@ -3170,16 +3163,16 @@
         <v>7524</v>
       </c>
       <c r="B120" s="33" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C120" s="34" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D120" s="35" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E120" s="38" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F120" s="29"/>
     </row>
@@ -3188,16 +3181,16 @@
         <v>7419</v>
       </c>
       <c r="B121" s="33" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C121" s="34" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D121" s="35" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="E121" s="38" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="F121" s="29"/>
     </row>
@@ -3206,52 +3199,54 @@
         <v>7420</v>
       </c>
       <c r="B122" s="33" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C122" s="34" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D122" s="35" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="E122" s="38" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="F122" s="29"/>
     </row>
-    <row r="123" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="37" t="n">
         <v>7525</v>
       </c>
       <c r="B123" s="33" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C123" s="34" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D123" s="35" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="E123" s="38" t="s">
-        <v>277</v>
-      </c>
-      <c r="F123" s="29"/>
+        <v>280</v>
+      </c>
+      <c r="F123" s="29" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="37" t="n">
         <v>7421</v>
       </c>
       <c r="B124" s="42" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="C124" s="43" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="D124" s="32" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="E124" s="38" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="F124" s="29"/>
     </row>
@@ -3262,7 +3257,7 @@
       <c r="B125" s="42"/>
       <c r="C125" s="43"/>
       <c r="D125" s="32" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E125" s="15"/>
       <c r="F125" s="29"/>
@@ -3272,16 +3267,16 @@
         <v>7422</v>
       </c>
       <c r="B126" s="42" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="C126" s="43" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="D126" s="32" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="E126" s="38" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="F126" s="29"/>
     </row>
@@ -3292,7 +3287,7 @@
       <c r="B127" s="42"/>
       <c r="C127" s="43"/>
       <c r="D127" s="32" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E127" s="15"/>
       <c r="F127" s="44"/>
@@ -3302,19 +3297,19 @@
         <v>7528</v>
       </c>
       <c r="B128" s="33" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C128" s="34" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D128" s="35" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E128" s="38" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="F128" s="29" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3322,16 +3317,16 @@
         <v>7450</v>
       </c>
       <c r="B129" s="33" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="C129" s="34" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="D129" s="33" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="E129" s="15" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="F129" s="29"/>
     </row>
@@ -3340,13 +3335,13 @@
         <v>7550</v>
       </c>
       <c r="B130" s="33" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="C130" s="34" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="D130" s="33" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="E130" s="15"/>
       <c r="F130" s="29"/>

</xml_diff>